<commit_message>
Create API input script matching template_v3.xlsm
</commit_message>
<xml_diff>
--- a/template_v3.xlsx
+++ b/template_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpollard/projects/comet/COMET-Farm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8668C17F-EFB5-3746-9B8A-D7EFE5520773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34865C72-78DF-A34C-A5CC-6009904B48B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
   </bookViews>
@@ -1569,7 +1569,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>

</xml_diff>